<commit_message>
Updated the .xls version of the progress file
</commit_message>
<xml_diff>
--- a/Documentation/Progress.xlsx
+++ b/Documentation/Progress.xlsx
@@ -9,22 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Progress" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -32,50 +27,80 @@
     <t>Highlights</t>
   </si>
   <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Next Steps</t>
+  </si>
+  <si>
     <t>Started interfacing pulse oximeter sensors available in the lab</t>
   </si>
   <si>
+    <t>Using Arduino UNO and MAX3501 Pulse Oximeter</t>
+  </si>
+  <si>
+    <t>Develop Arduino program for sensor control and data acquisition and transfer</t>
+  </si>
+  <si>
+    <t>Started sketching sensor holder prototype:</t>
+  </si>
+  <si>
+    <t>Forehead design</t>
+  </si>
+  <si>
+    <t>3D Design and printing of designs</t>
+  </si>
+  <si>
+    <t>Neck design</t>
+  </si>
+  <si>
     <t>Started building the data gathering, communication central</t>
   </si>
   <si>
-    <t>Started sketching sensor holder prototype:</t>
-  </si>
-  <si>
-    <t>Forehead design</t>
-  </si>
-  <si>
-    <t>Neck design</t>
-  </si>
-  <si>
-    <t>Next Steps</t>
+    <t>Python script, uses MQTT</t>
+  </si>
+  <si>
+    <t>Develop Python program for data transfer and logging</t>
   </si>
   <si>
     <t>Order parts as listed in proposal</t>
   </si>
   <si>
-    <t>3D Design and printing of designs</t>
-  </si>
-  <si>
-    <t>Develop Python program for data transfer and logging</t>
-  </si>
-  <si>
-    <t>Develop Arduino program for sensor control and data acquisition and transfer</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>Python script, uses MQTT</t>
-  </si>
-  <si>
-    <t>Using Arduino UNO and MAX3501 Pulse Oximeter</t>
+    <t>Continued interfacing pulse oximeter sensors available in the lab</t>
+  </si>
+  <si>
+    <t>Sensor does not seem to be performing as desired/expected</t>
+  </si>
+  <si>
+    <t>Using the PulseSensor from World Famous Electronics</t>
+  </si>
+  <si>
+    <t>Sensor performs on the Arduino, now adapting to the ESP32</t>
+  </si>
+  <si>
+    <t>Tested heart rate sensor for forehead, neck and earlobe</t>
+  </si>
+  <si>
+    <t>PulseSensor performs in every scenario</t>
+  </si>
+  <si>
+    <t>Build fixtures</t>
+  </si>
+  <si>
+    <t>Started design of three fixture models</t>
+  </si>
+  <si>
+    <t>Modelus are specific to forehead, neck, and earlobe</t>
+  </si>
+  <si>
+    <t>Will print models and test fixing to sensors, components</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,7 +109,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -93,13 +184,59 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,16 +245,226 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -140,39 +487,143 @@
       <right/>
       <top/>
       <bottom style="double">
-        <color indexed="64"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="1" builtinId="21"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -450,94 +901,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>43521</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4"/>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="6" t="s">
-        <v>8</v>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43550</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D4:D5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>